<commit_message>
Corrected last issues with Excel library...
* Publishing version 2.0.21.0
</commit_message>
<xml_diff>
--- a/Samples/SampleBook.xlsx
+++ b/Samples/SampleBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="14355" windowHeight="4680" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="14355" windowHeight="4680" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -149,6 +149,84 @@
   </si>
   <si>
     <t>Default cylinder</t>
+  </si>
+  <si>
+    <t>GALIC0040</t>
+  </si>
+  <si>
+    <t>300mm x 200mm x 90mm (ext) C40 - box with lid</t>
+  </si>
+  <si>
+    <t>GALIC0015</t>
+  </si>
+  <si>
+    <t>GALIC0014</t>
+  </si>
+  <si>
+    <t>GALIC0013</t>
+  </si>
+  <si>
+    <t>GALIC0012</t>
+  </si>
+  <si>
+    <t>GALIC0011</t>
+  </si>
+  <si>
+    <t>GALIC0010</t>
+  </si>
+  <si>
+    <t>GALIC0005</t>
+  </si>
+  <si>
+    <t>GALIC0016</t>
+  </si>
+  <si>
+    <t>300mm x 200mm x 200mm (ext) C15 - box without lid - 1440 pieces per Pallet</t>
+  </si>
+  <si>
+    <t>300mm x 200mm x 125mm (ext) C16 - box without lid - 1920 pieces per Pallet</t>
+  </si>
+  <si>
+    <t>400mm x 300mm x 150mm (ext) C14-box without lid - 480 pieces per Pallet</t>
+  </si>
+  <si>
+    <t>400mm x 300mm x 200mm (ext) C13-box without lid - 480 pieces per Pallet</t>
+  </si>
+  <si>
+    <t>400mm x 300mm x 300mm (ext) C12-box without lid - 480 pieces per Pallet</t>
+  </si>
+  <si>
+    <t>600mm x 400mm x 200mm (ext) C11-box without lid - 240 pieces per Pallet</t>
+  </si>
+  <si>
+    <t>600mm x 400mm x 250mm (ext) C10-box without lid - 240 pieces per Pallet</t>
+  </si>
+  <si>
+    <t>1000mm x 600mm x 500mm (ext) C5 box without lid - 150 pieces per Pallet</t>
+  </si>
+  <si>
+    <t>inter_CHEP AU</t>
+  </si>
+  <si>
+    <t>inter_UK Standard</t>
+  </si>
+  <si>
+    <t>inter_GMA 48x40</t>
+  </si>
+  <si>
+    <t>inter_CHEP NZ</t>
+  </si>
+  <si>
+    <t>inter_EUR</t>
+  </si>
+  <si>
+    <t>inter_EUR2</t>
+  </si>
+  <si>
+    <t>inter_EUR3</t>
+  </si>
+  <si>
+    <t>inter_EUR6</t>
   </si>
 </sst>
 </file>
@@ -515,16 +593,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -630,112 +708,292 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="6"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="8">
+        <v>300</v>
+      </c>
+      <c r="D4" s="8">
+        <v>200</v>
+      </c>
+      <c r="E4" s="8">
+        <v>90</v>
+      </c>
+      <c r="F4" s="8">
+        <v>294</v>
+      </c>
+      <c r="G4" s="8">
+        <v>194</v>
+      </c>
+      <c r="H4" s="8">
+        <v>84</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="6"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="8">
+        <v>300</v>
+      </c>
+      <c r="D5" s="8">
+        <v>200</v>
+      </c>
+      <c r="E5" s="8">
+        <v>200</v>
+      </c>
+      <c r="F5" s="8">
+        <v>294</v>
+      </c>
+      <c r="G5" s="8">
+        <v>194</v>
+      </c>
+      <c r="H5" s="8">
+        <v>194</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="6"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="8">
+        <v>300</v>
+      </c>
+      <c r="D6" s="8">
+        <v>200</v>
+      </c>
+      <c r="E6" s="8">
+        <v>125</v>
+      </c>
+      <c r="F6" s="8">
+        <v>294</v>
+      </c>
+      <c r="G6" s="8">
+        <v>194</v>
+      </c>
+      <c r="H6" s="8">
+        <v>119</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="6"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="8">
+        <v>400</v>
+      </c>
+      <c r="D7" s="8">
+        <v>300</v>
+      </c>
+      <c r="E7" s="8">
+        <v>150</v>
+      </c>
+      <c r="F7" s="8">
+        <v>394</v>
+      </c>
+      <c r="G7" s="8">
+        <v>294</v>
+      </c>
+      <c r="H7" s="8">
+        <v>144</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="6"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="8">
+        <v>400</v>
+      </c>
+      <c r="D8" s="8">
+        <v>300</v>
+      </c>
+      <c r="E8" s="8">
+        <v>200</v>
+      </c>
+      <c r="F8" s="8">
+        <v>394</v>
+      </c>
+      <c r="G8" s="8">
+        <v>294</v>
+      </c>
+      <c r="H8" s="8">
+        <v>194</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="6"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="8">
+        <v>400</v>
+      </c>
+      <c r="D9" s="8">
+        <v>300</v>
+      </c>
+      <c r="E9" s="8">
+        <v>300</v>
+      </c>
+      <c r="F9" s="8">
+        <v>394</v>
+      </c>
+      <c r="G9" s="8">
+        <v>294</v>
+      </c>
+      <c r="H9" s="8">
+        <v>294</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="6"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="8">
+        <v>600</v>
+      </c>
+      <c r="D10" s="8">
+        <v>400</v>
+      </c>
+      <c r="E10" s="8">
+        <v>200</v>
+      </c>
+      <c r="F10" s="8">
+        <v>594</v>
+      </c>
+      <c r="G10" s="8">
+        <v>394</v>
+      </c>
+      <c r="H10" s="8">
+        <v>194</v>
+      </c>
+      <c r="I10" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="6"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="8">
+        <v>600</v>
+      </c>
+      <c r="D11" s="8">
+        <v>400</v>
+      </c>
+      <c r="E11" s="8">
+        <v>250</v>
+      </c>
+      <c r="F11" s="8">
+        <v>594</v>
+      </c>
+      <c r="G11" s="8">
+        <v>394</v>
+      </c>
+      <c r="H11" s="8">
+        <v>244</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="6"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="8">
+        <v>600</v>
+      </c>
+      <c r="E12" s="8">
+        <v>500</v>
+      </c>
+      <c r="F12" s="8">
+        <v>990</v>
+      </c>
+      <c r="G12" s="8">
+        <v>590</v>
+      </c>
+      <c r="H12" s="8">
+        <v>490</v>
+      </c>
+      <c r="I12" s="9">
+        <v>1</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="6"/>
@@ -1757,42 +2015,6 @@
       <c r="I97" s="9"/>
       <c r="J97" s="9"/>
     </row>
-    <row r="98" spans="1:10">
-      <c r="A98" s="6"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8"/>
-      <c r="I98" s="9"/>
-      <c r="J98" s="9"/>
-    </row>
-    <row r="99" spans="1:10">
-      <c r="A99" s="6"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="8"/>
-      <c r="G99" s="8"/>
-      <c r="H99" s="8"/>
-      <c r="I99" s="9"/>
-      <c r="J99" s="9"/>
-    </row>
-    <row r="100" spans="1:10">
-      <c r="A100" s="6"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
-      <c r="G100" s="8"/>
-      <c r="H100" s="8"/>
-      <c r="I100" s="9"/>
-      <c r="J100" s="9"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1804,7 +2026,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4761,14 +4983,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4812,68 +5034,164 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1200</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1219.2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1016</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+      <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1165</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1165</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
+      <c r="A6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1200</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
+      <c r="A7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1200</v>
+      </c>
+      <c r="D7" s="8">
+        <v>800</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
+      <c r="A8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1200</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
+      <c r="A9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1200</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="8">
+        <v>800</v>
+      </c>
+      <c r="D10" s="8">
+        <v>600</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1"/>
@@ -6762,8 +7080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7599,5 +7917,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>